<commit_message>
Added Merit Lilin and Topica API / RTSP information
</commit_message>
<xml_diff>
--- a/ACTi/ACTi ISV Datasheet_camera.xlsx
+++ b/ACTi/ACTi ISV Datasheet_camera.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="120">
   <si>
     <t>Latest Firmware </t>
   </si>
@@ -101,7 +101,7 @@
     <t>CAM-5201</t>
   </si>
   <si>
-    <t>06&amp;07</t>
+    <t>720x480-30FPS,352x240-30FPS,160x112-30FPS</t>
   </si>
   <si>
     <t>1*DI,1*DO</t>
@@ -179,153 +179,156 @@
     <t>ACM-1011</t>
   </si>
   <si>
-    <t>08</t>
+    <t>640x480-30FPS,352x240-30FPS,160x112-30FPS</t>
   </si>
   <si>
     <t>ACM-1231</t>
   </si>
   <si>
+    <t>1280x1024-18FPS,1280x720-26FPS,640x480-30FPS,320x240-30FPS,160x112-30FPS</t>
+  </si>
+  <si>
+    <t>ACM-1232</t>
+  </si>
+  <si>
     <t>01</t>
   </si>
   <si>
-    <t>ACM-1232</t>
-  </si>
-  <si>
     <t>ACM-1311</t>
   </si>
   <si>
+    <t>ACM-1431</t>
+  </si>
+  <si>
+    <t>ACM-1432</t>
+  </si>
+  <si>
+    <t>ACM-1511</t>
+  </si>
+  <si>
+    <t>IP Dome Camera</t>
+  </si>
+  <si>
+    <t>ACM-3001</t>
+  </si>
+  <si>
+    <t>ACM-3011</t>
+  </si>
+  <si>
+    <t>ACM-3211</t>
+  </si>
+  <si>
+    <t>ACM-3311</t>
+  </si>
+  <si>
+    <t>ACM-3401</t>
+  </si>
+  <si>
+    <t>ACM-3411</t>
+  </si>
+  <si>
+    <t>ACM-3511</t>
+  </si>
+  <si>
+    <t>ACM-3601</t>
+  </si>
+  <si>
+    <t>RJ45 connector</t>
+  </si>
+  <si>
+    <t>ACM-3603</t>
+  </si>
+  <si>
+    <t>M12 connector</t>
+  </si>
+  <si>
+    <t>ACM-3701</t>
+  </si>
+  <si>
+    <t>ACM-3703</t>
+  </si>
+  <si>
+    <t>ACM-7411</t>
+  </si>
+  <si>
+    <t>ACM-7511</t>
+  </si>
+  <si>
+    <t>IP Cube Camera</t>
+  </si>
+  <si>
+    <t>ACM-4000</t>
+  </si>
+  <si>
+    <t>ACM-4200</t>
+  </si>
+  <si>
+    <t>ACM-4201</t>
+  </si>
+  <si>
+    <t>IP Box Camera</t>
+  </si>
+  <si>
+    <t>ACM-5001</t>
+  </si>
+  <si>
+    <t>ACM-5601</t>
+  </si>
+  <si>
+    <t>ACM-5611</t>
+  </si>
+  <si>
+    <t>ACM-5711</t>
+  </si>
+  <si>
+    <t>PTZ Camera</t>
+  </si>
+  <si>
+    <t>ACM-8201</t>
+  </si>
+  <si>
+    <t>ACM-8211</t>
+  </si>
+  <si>
+    <t>ACM-8511</t>
+  </si>
+  <si>
+    <t>ACD-2100</t>
+  </si>
+  <si>
+    <t>2.06.00+  3.11.13</t>
+  </si>
+  <si>
+    <t>Video Server(4ch)</t>
+  </si>
+  <si>
+    <t>ACD-2200</t>
+  </si>
+  <si>
+    <t>Video Server(8ch)</t>
+  </si>
+  <si>
+    <t>ACD-2300</t>
+  </si>
+  <si>
+    <t>Video Server(16ch)</t>
+  </si>
+  <si>
+    <t>ACD-2400</t>
+  </si>
+  <si>
+    <t>3.02.06</t>
+  </si>
+  <si>
+    <t>Decoder</t>
+  </si>
+  <si>
+    <t>ACD-3100</t>
+  </si>
+  <si>
     <t>02&amp;03</t>
   </si>
   <si>
-    <t>ACM-1431</t>
-  </si>
-  <si>
-    <t>ACM-1432</t>
-  </si>
-  <si>
-    <t>ACM-1511</t>
-  </si>
-  <si>
-    <t>IP Dome Camera</t>
-  </si>
-  <si>
-    <t>ACM-3001</t>
-  </si>
-  <si>
-    <t>ACM-3011</t>
-  </si>
-  <si>
-    <t>ACM-3211</t>
-  </si>
-  <si>
-    <t>ACM-3311</t>
-  </si>
-  <si>
-    <t>ACM-3401</t>
-  </si>
-  <si>
-    <t>ACM-3411</t>
-  </si>
-  <si>
-    <t>ACM-3511</t>
-  </si>
-  <si>
-    <t>ACM-3601</t>
-  </si>
-  <si>
-    <t>RJ45 connector</t>
-  </si>
-  <si>
-    <t>ACM-3603</t>
-  </si>
-  <si>
-    <t>M12 connector</t>
-  </si>
-  <si>
-    <t>ACM-3701</t>
-  </si>
-  <si>
-    <t>ACM-3703</t>
-  </si>
-  <si>
-    <t>ACM-7411</t>
-  </si>
-  <si>
-    <t>ACM-7511</t>
-  </si>
-  <si>
-    <t>IP Cube Camera</t>
-  </si>
-  <si>
-    <t>ACM-4000</t>
-  </si>
-  <si>
-    <t>ACM-4200</t>
-  </si>
-  <si>
-    <t>ACM-4201</t>
-  </si>
-  <si>
-    <t>IP Box Camera</t>
-  </si>
-  <si>
-    <t>ACM-5001</t>
-  </si>
-  <si>
-    <t>ACM-5601</t>
-  </si>
-  <si>
-    <t>ACM-5611</t>
-  </si>
-  <si>
-    <t>ACM-5711</t>
-  </si>
-  <si>
-    <t>PTZ Camera</t>
-  </si>
-  <si>
-    <t>ACM-8201</t>
-  </si>
-  <si>
-    <t>ACM-8211</t>
-  </si>
-  <si>
-    <t>ACM-8511</t>
-  </si>
-  <si>
-    <t>ACD-2100</t>
-  </si>
-  <si>
-    <t>2.06.00+  3.11.13</t>
-  </si>
-  <si>
-    <t>Video Server(4ch)</t>
-  </si>
-  <si>
-    <t>ACD-2200</t>
-  </si>
-  <si>
-    <t>Video Server(8ch)</t>
-  </si>
-  <si>
-    <t>ACD-2300</t>
-  </si>
-  <si>
-    <t>Video Server(16ch)</t>
-  </si>
-  <si>
-    <t>ACD-2400</t>
-  </si>
-  <si>
-    <t>3.02.06</t>
-  </si>
-  <si>
-    <t>Decoder</t>
-  </si>
-  <si>
-    <t>ACD-3100</t>
-  </si>
-  <si>
     <t>3.03.02</t>
   </si>
   <si>
@@ -347,6 +350,9 @@
     <t>TCM-1232</t>
   </si>
   <si>
+    <t>1280x1024,1280x720,640x480,320x240,160x112</t>
+  </si>
+  <si>
     <t>TCM-1511</t>
   </si>
   <si>
@@ -371,7 +377,7 @@
     <t>TCM-5311</t>
   </si>
   <si>
-    <t>09</t>
+    <t>1280x960,1280x720,640x480,320x240,160x112</t>
   </si>
   <si>
     <t>TCM-5312</t>
@@ -623,7 +629,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
@@ -698,6 +704,9 @@
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="true" textRotation="0" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
@@ -760,8 +769,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/vmlDrawing1.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?>
-<xml xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:x="urn:schemas-microsoft-com:office:excel"><v:shapetype id="shapetype_75" coordsize="21600,21600" o:spt="75" adj="2700" path="m,l21600,l21600,21600l,21600xm@0@0l@0@2l@1@2l@1@0xe"><v:stroke joinstyle="miter"/><v:formulas><v:f eqn="val #0"/><v:f eqn="sum width 0 @0"/><v:f eqn="sum height 0 @0"/></v:formulas><v:path gradientshapeok="t" o:connecttype="rect" textboxrect="@0,@0,@1,@2"/><v:handles><v:h position="@0,0"/></v:handles></v:shapetype><v:shape id="shape_32564" style="position:absolute;margin-left:1240pt;margin-top:132.45pt;width:127.4pt;height:46.5pt;visibility:hidden" type="shapetype_75"><w10:wrap w10:type="none"/><v:fill color="#ffffe1" color2="#00001e" detectmouseclick="t" type="solid"/><v:stroke color="black" joinstyle="miter" startarrow="block" startarrowlength="medium" startarrowwidth="medium"/><x:ClientData ObjectType="Note"><x:MoveWithCells/><x:SizeWithCells/><x:Anchor>2, 15, 0, 15, 4, 31, 4, 21</x:Anchor><x:AutoFill>False</x:AutoFill><x:Row>8</x:Row><x:Column>11</x:Column></x:ClientData></v:shape></xml>
+<file path=xl/drawings/vmlDrawing2.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?>
+<xml xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:x="urn:schemas-microsoft-com:office:excel"><v:shapetype id="shapetype_75" coordsize="21600,21600" o:spt="75" adj="2700" path="m,l21600,l21600,21600l,21600xm@0@0l@0@2l@1@2l@1@0xe"><v:stroke joinstyle="miter"/><v:formulas><v:f eqn="val #0"/><v:f eqn="sum width 0 @0"/><v:f eqn="sum height 0 @0"/></v:formulas><v:path gradientshapeok="t" o:connecttype="rect" textboxrect="@0,@0,@1,@2"/><v:handles><v:h position="@0,0"/></v:handles></v:shapetype><v:shape id="shape_32564" style="position:absolute;margin-left:1747.1pt;margin-top:132.45pt;width:127.4pt;height:46.5pt;visibility:hidden" type="shapetype_75"><w10:wrap w10:type="none"/><v:fill color="#ffffe1" color2="#00001e" detectmouseclick="t" type="solid"/><v:stroke color="black" joinstyle="miter" startarrow="block" startarrowlength="medium" startarrowwidth="medium"/><x:ClientData ObjectType="Note"><x:MoveWithCells/><x:SizeWithCells/><x:Anchor>2, 15, 0, 15, 4, 31, 4, 21</x:Anchor><x:AutoFill>False</x:AutoFill><x:Row>8</x:Row><x:Column>11</x:Column></x:ClientData></v:shape></xml>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -780,7 +789,8 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8823529411765"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6352941176471"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.878431372549"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="12.878431372549"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="79.678431372549"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.878431372549"/>
     <col collapsed="false" hidden="false" max="9" min="7" style="0" width="12.6313725490196"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.7607843137255"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.878431372549"/>
@@ -1282,7 +1292,7 @@
       <c r="D18" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="31" t="s">
         <v>50</v>
       </c>
       <c r="F18" s="11"/>
@@ -1307,7 +1317,7 @@
         <v>51</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="17"/>
@@ -1328,10 +1338,10 @@
       <c r="B20" s="29"/>
       <c r="C20" s="30"/>
       <c r="D20" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="17"/>
@@ -1355,7 +1365,7 @@
         <v>54</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="17"/>
@@ -1379,7 +1389,7 @@
         <v>55</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="17"/>
@@ -1403,7 +1413,7 @@
         <v>56</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="17"/>
@@ -1452,10 +1462,10 @@
       <c r="D25" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F25" s="31"/>
+      <c r="F25" s="32"/>
       <c r="G25" s="17"/>
       <c r="H25" s="17"/>
       <c r="I25" s="16"/>
@@ -1477,7 +1487,7 @@
         <v>60</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="17"/>
@@ -1501,7 +1511,7 @@
         <v>61</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="17"/>
@@ -1525,7 +1535,7 @@
         <v>62</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F28" s="11"/>
       <c r="G28" s="17"/>
@@ -1549,7 +1559,7 @@
         <v>63</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F29" s="11"/>
       <c r="G29" s="17"/>
@@ -1572,10 +1582,10 @@
       <c r="D30" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E30" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="F30" s="31"/>
+      <c r="E30" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="F30" s="32"/>
       <c r="G30" s="17"/>
       <c r="H30" s="17"/>
       <c r="I30" s="16"/>
@@ -1596,10 +1606,10 @@
       <c r="D31" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="31" t="s">
+      <c r="E31" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F31" s="31"/>
+      <c r="F31" s="32"/>
       <c r="G31" s="17"/>
       <c r="H31" s="17"/>
       <c r="I31" s="16"/>
@@ -1624,10 +1634,10 @@
       <c r="D32" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E32" s="31" t="s">
+      <c r="E32" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F32" s="31"/>
+      <c r="F32" s="32"/>
       <c r="G32" s="17"/>
       <c r="H32" s="17"/>
       <c r="I32" s="16"/>
@@ -1650,10 +1660,10 @@
       <c r="D33" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E33" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="F33" s="31"/>
+      <c r="E33" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="F33" s="32"/>
       <c r="G33" s="17"/>
       <c r="H33" s="17"/>
       <c r="I33" s="16"/>
@@ -1676,10 +1686,10 @@
       <c r="D34" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E34" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="F34" s="31"/>
+      <c r="E34" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="F34" s="32"/>
       <c r="G34" s="17"/>
       <c r="H34" s="17"/>
       <c r="I34" s="16"/>
@@ -1703,7 +1713,7 @@
         <v>71</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F35" s="12" t="s">
         <v>23</v>
@@ -1729,7 +1739,7 @@
         <v>72</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="F36" s="12" t="s">
         <v>23</v>
@@ -1757,7 +1767,7 @@
         <v>74</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="F37" s="11"/>
       <c r="G37" s="17"/>
@@ -1785,7 +1795,7 @@
         <v>75</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F38" s="11"/>
       <c r="G38" s="17"/>
@@ -1809,7 +1819,7 @@
         <v>76</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F39" s="11"/>
       <c r="G39" s="17"/>
@@ -1861,7 +1871,7 @@
         <v>79</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F41" s="12" t="s">
         <v>23</v>
@@ -1887,7 +1897,7 @@
         <v>80</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F42" s="12" t="s">
         <v>23</v>
@@ -1913,7 +1923,7 @@
         <v>81</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="F43" s="12" t="s">
         <v>23</v>
@@ -1934,14 +1944,14 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.2" outlineLevel="0" r="44">
       <c r="A44" s="7"/>
       <c r="B44" s="29"/>
-      <c r="C44" s="32" t="s">
+      <c r="C44" s="33" t="s">
         <v>82</v>
       </c>
       <c r="D44" s="10" t="s">
         <v>83</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F44" s="12" t="s">
         <v>23</v>
@@ -1962,12 +1972,12 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.2" outlineLevel="0" r="45">
       <c r="A45" s="7"/>
       <c r="B45" s="29"/>
-      <c r="C45" s="32"/>
+      <c r="C45" s="33"/>
       <c r="D45" s="10" t="s">
         <v>84</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F45" s="12" t="s">
         <v>23</v>
@@ -1988,12 +1998,12 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.2" outlineLevel="0" r="46">
       <c r="A46" s="7"/>
       <c r="B46" s="29"/>
-      <c r="C46" s="32"/>
+      <c r="C46" s="33"/>
       <c r="D46" s="10" t="s">
         <v>85</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="F46" s="12" t="s">
         <v>23</v>
@@ -2021,7 +2031,7 @@
         <v>86</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="F47" s="12" t="s">
         <v>39</v>
@@ -2051,7 +2061,7 @@
         <v>89</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="F48" s="12" t="s">
         <v>39</v>
@@ -2079,7 +2089,7 @@
         <v>91</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="F49" s="12" t="s">
         <v>39</v>
@@ -2107,7 +2117,7 @@
         <v>93</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="F50" s="12" t="s">
         <v>39</v>
@@ -2125,19 +2135,19 @@
       <c r="Q50" s="17"/>
       <c r="R50" s="18"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="51">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="51">
       <c r="A51" s="7"/>
-      <c r="B51" s="33" t="s">
+      <c r="B51" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="C51" s="34" t="s">
+      <c r="C51" s="35" t="s">
         <v>95</v>
       </c>
       <c r="D51" s="10" t="s">
         <v>96</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="F51" s="12"/>
       <c r="G51" s="17"/>
@@ -2153,19 +2163,19 @@
       <c r="Q51" s="17"/>
       <c r="R51" s="18"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.2" outlineLevel="0" r="52">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.85" outlineLevel="0" r="52">
       <c r="A52" s="7"/>
-      <c r="B52" s="35" t="s">
-        <v>97</v>
+      <c r="B52" s="36" t="s">
+        <v>98</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>53</v>
+        <v>100</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="F52" s="12" t="s">
         <v>39</v>
@@ -2184,33 +2194,33 @@
       <c r="R52" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.2" outlineLevel="0" r="53">
-      <c r="D53" s="36"/>
-      <c r="E53" s="37"/>
-      <c r="F53" s="37"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="36"/>
-      <c r="I53" s="36"/>
-      <c r="J53" s="37"/>
-      <c r="K53" s="37"/>
-      <c r="L53" s="36"/>
-      <c r="M53" s="36"/>
-      <c r="N53" s="36"/>
-      <c r="O53" s="36"/>
-      <c r="P53" s="36"/>
-      <c r="Q53" s="36"/>
+      <c r="D53" s="37"/>
+      <c r="E53" s="38"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="37"/>
+      <c r="J53" s="38"/>
+      <c r="K53" s="38"/>
+      <c r="L53" s="37"/>
+      <c r="M53" s="37"/>
+      <c r="N53" s="37"/>
+      <c r="O53" s="37"/>
+      <c r="P53" s="37"/>
+      <c r="Q53" s="37"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.2" outlineLevel="0" r="54">
       <c r="A54" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B54" s="29" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C54" s="30" t="s">
         <v>46</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E54" s="12" t="s">
         <v>50</v>
@@ -2238,10 +2248,10 @@
       <c r="B55" s="29"/>
       <c r="C55" s="30"/>
       <c r="D55" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="F55" s="12" t="s">
         <v>23</v>
@@ -2264,10 +2274,10 @@
       <c r="B56" s="29"/>
       <c r="C56" s="30"/>
       <c r="D56" s="10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="F56" s="12" t="s">
         <v>23</v>
@@ -2292,10 +2302,10 @@
         <v>57</v>
       </c>
       <c r="D57" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E57" s="12" t="s">
         <v>105</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>50</v>
       </c>
       <c r="F57" s="12" t="s">
         <v>23</v>
@@ -2318,10 +2328,10 @@
       <c r="B58" s="29"/>
       <c r="C58" s="30"/>
       <c r="D58" s="10" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="F58" s="12" t="s">
         <v>23</v>
@@ -2344,10 +2354,10 @@
       <c r="B59" s="29"/>
       <c r="C59" s="30"/>
       <c r="D59" s="10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="F59" s="12" t="s">
         <v>23</v>
@@ -2370,10 +2380,10 @@
       <c r="B60" s="29"/>
       <c r="C60" s="30"/>
       <c r="D60" s="10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="F60" s="12" t="s">
         <v>23</v>
@@ -2391,17 +2401,17 @@
       <c r="Q60" s="17"/>
       <c r="R60" s="18"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.2" outlineLevel="0" r="61">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.85" outlineLevel="0" r="61">
       <c r="A61" s="7"/>
       <c r="B61" s="29"/>
-      <c r="C61" s="38" t="s">
-        <v>109</v>
+      <c r="C61" s="39" t="s">
+        <v>111</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="F61" s="12"/>
       <c r="G61" s="17"/>
@@ -2428,10 +2438,10 @@
         <v>77</v>
       </c>
       <c r="D62" s="17" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F62" s="12" t="s">
         <v>23</v>
@@ -2454,10 +2464,10 @@
       <c r="B63" s="29"/>
       <c r="C63" s="30"/>
       <c r="D63" s="17" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F63" s="12" t="s">
         <v>23</v>
@@ -2480,10 +2490,10 @@
       <c r="B64" s="29"/>
       <c r="C64" s="30"/>
       <c r="D64" s="17" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="F64" s="12" t="s">
         <v>23</v>
@@ -2506,10 +2516,10 @@
       <c r="B65" s="29"/>
       <c r="C65" s="30"/>
       <c r="D65" s="17" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="F65" s="12" t="s">
         <v>23</v>
@@ -2527,62 +2537,62 @@
       <c r="Q65" s="17"/>
       <c r="R65" s="18"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.2" outlineLevel="0" r="66">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.85" outlineLevel="0" r="66">
       <c r="A66" s="7"/>
       <c r="B66" s="29"/>
-      <c r="C66" s="39" t="s">
+      <c r="C66" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="D66" s="40" t="s">
-        <v>116</v>
-      </c>
-      <c r="E66" s="41" t="s">
-        <v>53</v>
+      <c r="D66" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="F66" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G66" s="40"/>
-      <c r="H66" s="40"/>
-      <c r="I66" s="40"/>
-      <c r="J66" s="41"/>
-      <c r="K66" s="41"/>
-      <c r="L66" s="40"/>
-      <c r="M66" s="40"/>
-      <c r="N66" s="40"/>
-      <c r="O66" s="40"/>
-      <c r="P66" s="40"/>
-      <c r="Q66" s="40"/>
-      <c r="R66" s="42"/>
+      <c r="G66" s="41"/>
+      <c r="H66" s="41"/>
+      <c r="I66" s="41"/>
+      <c r="J66" s="42"/>
+      <c r="K66" s="42"/>
+      <c r="L66" s="41"/>
+      <c r="M66" s="41"/>
+      <c r="N66" s="41"/>
+      <c r="O66" s="41"/>
+      <c r="P66" s="41"/>
+      <c r="Q66" s="41"/>
+      <c r="R66" s="43"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.2" outlineLevel="0" r="67">
-      <c r="A67" s="43"/>
-      <c r="B67" s="44"/>
-      <c r="C67" s="45"/>
-      <c r="D67" s="46"/>
-      <c r="E67" s="47"/>
-      <c r="F67" s="44"/>
-      <c r="G67" s="45"/>
-      <c r="H67" s="45"/>
-      <c r="I67" s="45"/>
-      <c r="J67" s="44"/>
-      <c r="K67" s="44"/>
-      <c r="L67" s="45"/>
-      <c r="M67" s="45"/>
-      <c r="N67" s="45"/>
-      <c r="O67" s="45"/>
-      <c r="P67" s="45"/>
-      <c r="Q67" s="45"/>
-      <c r="R67" s="48"/>
+      <c r="A67" s="44"/>
+      <c r="B67" s="45"/>
+      <c r="C67" s="46"/>
+      <c r="D67" s="47"/>
+      <c r="E67" s="48"/>
+      <c r="F67" s="45"/>
+      <c r="G67" s="46"/>
+      <c r="H67" s="46"/>
+      <c r="I67" s="46"/>
+      <c r="J67" s="45"/>
+      <c r="K67" s="45"/>
+      <c r="L67" s="46"/>
+      <c r="M67" s="46"/>
+      <c r="N67" s="46"/>
+      <c r="O67" s="46"/>
+      <c r="P67" s="46"/>
+      <c r="Q67" s="46"/>
+      <c r="R67" s="49"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="141" outlineLevel="0" r="68">
-      <c r="C68" s="49" t="s">
-        <v>117</v>
-      </c>
-      <c r="D68" s="49"/>
-      <c r="E68" s="49"/>
-      <c r="F68" s="50"/>
-      <c r="I68" s="51"/>
+      <c r="C68" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="D68" s="50"/>
+      <c r="E68" s="50"/>
+      <c r="F68" s="51"/>
+      <c r="I68" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="33">

</xml_diff>